<commit_message>
Stupid fix: Garanti nepřednášejí
Nejstupidnější způsob jak to šlo

- Explodni ID garantů
- Zjisti zda jsou individuální id v seznamu přednášejících
- Agreguj řádky podle katedry + zkratky,  vypiš do sloupce neobsažená id

MUSÍ to jít líp
</commit_message>
<xml_diff>
--- a/results_xlsx/bez_garanta.xlsx
+++ b/results_xlsx/bez_garanta.xlsx
@@ -475,12 +475,12 @@
     <t>Úvod do molekulárních simulací</t>
   </si>
   <si>
+    <t>Bakalářská práce z fyziky</t>
+  </si>
+  <si>
     <t>Bakalářská práce z chemie</t>
   </si>
   <si>
-    <t>Bakalářská práce z fyziky</t>
-  </si>
-  <si>
     <t>PVK - Elektronika II</t>
   </si>
   <si>
@@ -493,18 +493,18 @@
     <t>PVK - Mikroprocesorová technika</t>
   </si>
   <si>
+    <t>PVK - Automatizované měřící systémy</t>
+  </si>
+  <si>
     <t>Biochemická cvičení</t>
   </si>
   <si>
-    <t>PVK - Automatizované měřící systémy</t>
+    <t>Diplomová práce z chemie</t>
   </si>
   <si>
     <t>Diplomová práce fyziky</t>
   </si>
   <si>
-    <t>Diplomová práce z chemie</t>
-  </si>
-  <si>
     <t>Obecná botanika</t>
   </si>
   <si>
@@ -571,60 +571,60 @@
     <t>Anglický jazyk pro doktorandy</t>
   </si>
   <si>
+    <t>SZZ - biologie s didaktikou</t>
+  </si>
+  <si>
+    <t>SZZ - Geografie s didaktikou</t>
+  </si>
+  <si>
     <t>SZZ - matematika s didaktikou</t>
   </si>
   <si>
-    <t>SZZ - biologie s didaktikou</t>
-  </si>
-  <si>
-    <t>SZZ - Geografie s didaktikou</t>
-  </si>
-  <si>
     <t>Biologie</t>
   </si>
   <si>
     <t>Softwarové systémy</t>
   </si>
   <si>
+    <t>Aplikovaná fyzika</t>
+  </si>
+  <si>
     <t>Aplikovaná geografie - Cestovní ruch</t>
   </si>
   <si>
-    <t>Aplikovaná fyzika</t>
+    <t>Nanotechnologie</t>
+  </si>
+  <si>
+    <t>Informační technologie</t>
   </si>
   <si>
     <t>Aplikovaná geografie - Krajina a GIS</t>
   </si>
   <si>
-    <t>Nanotechnologie</t>
-  </si>
-  <si>
-    <t>Informační technologie</t>
-  </si>
-  <si>
     <t>Matematika s aplikacemi</t>
   </si>
   <si>
+    <t>SZZ - Evropská integrace a EU</t>
+  </si>
+  <si>
     <t>Počítačové modelování</t>
   </si>
   <si>
-    <t>SZZ - Evropská integrace a EU</t>
-  </si>
-  <si>
     <t>SZZ - Chemie</t>
   </si>
   <si>
     <t>Statistika a zpracování dat</t>
   </si>
   <si>
+    <t>Biologie s didaktikou pro SŠ</t>
+  </si>
+  <si>
+    <t>Chemie a didaktika chemie pro SŠ</t>
+  </si>
+  <si>
     <t>Geografie krajiny a GIS</t>
   </si>
   <si>
-    <t>Chemie a didaktika chemie pro SŠ</t>
-  </si>
-  <si>
-    <t>Biologie s didaktikou pro SŠ</t>
-  </si>
-  <si>
     <t>SZZ - Fyzika s didaktikou pro SŠ</t>
   </si>
   <si>
@@ -634,28 +634,31 @@
     <t>Regionální geografie a cestovní ruch</t>
   </si>
   <si>
+    <t>SZZ - numerická matematika</t>
+  </si>
+  <si>
     <t>SZZ - Reg. geografie a reg. rozvoj Česka</t>
   </si>
   <si>
-    <t>SZZ - numerická matematika</t>
-  </si>
-  <si>
     <t>SZZ - Toxikologie a analýza škodlivin</t>
   </si>
   <si>
+    <t>Geografie pro vzdělávání</t>
+  </si>
+  <si>
+    <t>Chemie pro vzdělávání</t>
+  </si>
+  <si>
+    <t>Matematika pro vzdělávání</t>
+  </si>
+  <si>
+    <t>Biologie pro vzdělávání</t>
+  </si>
+  <si>
     <t>Fyzika pro vzdělávání</t>
   </si>
   <si>
-    <t>Geografie pro vzdělávání</t>
-  </si>
-  <si>
-    <t>Chemie pro vzdělávání</t>
-  </si>
-  <si>
-    <t>Matematika pro vzdělávání</t>
-  </si>
-  <si>
-    <t>Biologie pro vzdělávání</t>
+    <t>Analytická chemie</t>
   </si>
   <si>
     <t>SZZ - Biologie</t>
@@ -664,18 +667,15 @@
     <t>Fyzika</t>
   </si>
   <si>
-    <t>Analytická chemie</t>
-  </si>
-  <si>
     <t>SZZ- Regionální geografie Evropy a světa</t>
   </si>
   <si>
+    <t>Toxikologie</t>
+  </si>
+  <si>
     <t>Matematika s didaktikou pro ZŠ</t>
   </si>
   <si>
-    <t>Toxikologie</t>
-  </si>
-  <si>
     <t>Matematika s didaktikou pro SŠ</t>
   </si>
   <si>
@@ -688,21 +688,21 @@
     <t>SZZ - Informatika</t>
   </si>
   <si>
+    <t>Chemie</t>
+  </si>
+  <si>
     <t>Matematika</t>
   </si>
   <si>
-    <t>Chemie</t>
+    <t>Matematická informatika</t>
+  </si>
+  <si>
+    <t>SZZ - Obecná geografie</t>
   </si>
   <si>
     <t>Elektronika a elektrotechnika</t>
   </si>
   <si>
-    <t>Matematická informatika</t>
-  </si>
-  <si>
-    <t>SZZ - Obecná geografie</t>
-  </si>
-  <si>
     <t>SZZ - Sociální geografie</t>
   </si>
   <si>
@@ -751,24 +751,24 @@
     <t>Sociální geografie a územní rozvoj</t>
   </si>
   <si>
+    <t>Učitelství biologie pro střední školy</t>
+  </si>
+  <si>
+    <t>Učitelství fyziky pro střední školy</t>
+  </si>
+  <si>
     <t>Učitelství chemie pro střední školy</t>
   </si>
   <si>
-    <t>Učitelství biologie pro střední školy</t>
+    <t>Učitelství geografie pro střední školy</t>
+  </si>
+  <si>
+    <t>Učitelství informatiky pro střední školy</t>
   </si>
   <si>
     <t>Učitelství matematiky pro střední školy</t>
   </si>
   <si>
-    <t>Učitelství geografie pro střední školy</t>
-  </si>
-  <si>
-    <t>Učitelství fyziky pro střední školy</t>
-  </si>
-  <si>
-    <t>Učitelství informatiky pro střední školy</t>
-  </si>
-  <si>
     <t>Teoretické základy datového inženýrství</t>
   </si>
   <si>
@@ -820,15 +820,15 @@
     <t>Chemické inženýrství</t>
   </si>
   <si>
+    <t>Biologie s didaktikou</t>
+  </si>
+  <si>
+    <t>Geografie s didaktikou pro ZŠ</t>
+  </si>
+  <si>
     <t>Matematika s didaktikou</t>
   </si>
   <si>
-    <t>Biologie s didaktikou</t>
-  </si>
-  <si>
-    <t>Geografie s didaktikou pro ZŠ</t>
-  </si>
-  <si>
     <t>Geografie s didaktikou pro SŠ</t>
   </si>
   <si>
@@ -838,10 +838,10 @@
     <t>Fyzika s didaktikou pro SŠ</t>
   </si>
   <si>
+    <t>Numerická matematika</t>
+  </si>
+  <si>
     <t>Regionální geografie a regionální rozvoj Česka</t>
-  </si>
-  <si>
-    <t>Numerická matematika</t>
   </si>
   <si>
     <t>Toxikologie a analýza škodlivin</t>
@@ -1495,7 +1495,7 @@
     </row>
     <row r="14" spans="1:7">
       <c r="A14" s="1" t="s">
-        <v>8</v>
+        <v>10</v>
       </c>
       <c r="B14" s="1" t="s">
         <v>27</v>
@@ -1514,7 +1514,7 @@
     </row>
     <row r="15" spans="1:7">
       <c r="A15" s="1" t="s">
-        <v>12</v>
+        <v>8</v>
       </c>
       <c r="B15" s="1" t="s">
         <v>27</v>
@@ -1533,7 +1533,7 @@
     </row>
     <row r="16" spans="1:7">
       <c r="A16" s="1" t="s">
-        <v>10</v>
+        <v>12</v>
       </c>
       <c r="B16" s="1" t="s">
         <v>27</v>
@@ -1552,7 +1552,7 @@
     </row>
     <row r="17" spans="1:7">
       <c r="A17" s="1" t="s">
-        <v>13</v>
+        <v>8</v>
       </c>
       <c r="B17" s="1" t="s">
         <v>28</v>
@@ -1571,7 +1571,7 @@
     </row>
     <row r="18" spans="1:7">
       <c r="A18" s="1" t="s">
-        <v>8</v>
+        <v>13</v>
       </c>
       <c r="B18" s="1" t="s">
         <v>28</v>
@@ -1590,7 +1590,7 @@
     </row>
     <row r="19" spans="1:7">
       <c r="A19" s="1" t="s">
-        <v>13</v>
+        <v>8</v>
       </c>
       <c r="B19" s="1" t="s">
         <v>29</v>
@@ -1609,7 +1609,7 @@
     </row>
     <row r="20" spans="1:7">
       <c r="A20" s="1" t="s">
-        <v>8</v>
+        <v>13</v>
       </c>
       <c r="B20" s="1" t="s">
         <v>29</v>
@@ -1761,7 +1761,7 @@
     </row>
     <row r="28" spans="1:7">
       <c r="A28" s="1" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
       <c r="B28" s="1" t="s">
         <v>35</v>
@@ -1780,7 +1780,7 @@
     </row>
     <row r="29" spans="1:7">
       <c r="A29" s="1" t="s">
-        <v>11</v>
+        <v>12</v>
       </c>
       <c r="B29" s="1" t="s">
         <v>35</v>
@@ -2008,7 +2008,7 @@
     </row>
     <row r="41" spans="1:7">
       <c r="A41" s="1" t="s">
-        <v>10</v>
+        <v>8</v>
       </c>
       <c r="B41" s="1" t="s">
         <v>47</v>
@@ -2027,7 +2027,7 @@
     </row>
     <row r="42" spans="1:7">
       <c r="A42" s="1" t="s">
-        <v>8</v>
+        <v>10</v>
       </c>
       <c r="B42" s="1" t="s">
         <v>47</v>
@@ -2141,7 +2141,7 @@
     </row>
     <row r="48" spans="1:7">
       <c r="A48" s="1" t="s">
-        <v>10</v>
+        <v>8</v>
       </c>
       <c r="B48" s="1" t="s">
         <v>53</v>
@@ -2153,14 +2153,14 @@
         <v>159</v>
       </c>
       <c r="E48" s="1" t="s">
-        <v>159</v>
+        <v>265</v>
       </c>
       <c r="F48" s="1"/>
       <c r="G48" s="1"/>
     </row>
     <row r="49" spans="1:7">
       <c r="A49" s="1" t="s">
-        <v>8</v>
+        <v>10</v>
       </c>
       <c r="B49" s="1" t="s">
         <v>53</v>
@@ -2172,14 +2172,14 @@
         <v>160</v>
       </c>
       <c r="E49" s="1" t="s">
-        <v>265</v>
+        <v>160</v>
       </c>
       <c r="F49" s="1"/>
       <c r="G49" s="1"/>
     </row>
     <row r="50" spans="1:7">
       <c r="A50" s="1" t="s">
-        <v>8</v>
+        <v>10</v>
       </c>
       <c r="B50" s="1" t="s">
         <v>54</v>
@@ -2191,14 +2191,14 @@
         <v>161</v>
       </c>
       <c r="E50" s="1" t="s">
-        <v>141</v>
+        <v>161</v>
       </c>
       <c r="F50" s="1"/>
       <c r="G50" s="1"/>
     </row>
     <row r="51" spans="1:7">
       <c r="A51" s="1" t="s">
-        <v>10</v>
+        <v>8</v>
       </c>
       <c r="B51" s="1" t="s">
         <v>54</v>
@@ -2210,7 +2210,7 @@
         <v>162</v>
       </c>
       <c r="E51" s="1" t="s">
-        <v>162</v>
+        <v>141</v>
       </c>
       <c r="F51" s="1"/>
       <c r="G51" s="1"/>
@@ -2730,7 +2730,7 @@
     </row>
     <row r="79" spans="1:7">
       <c r="A79" s="1" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="B79" s="1" t="s">
         <v>81</v>
@@ -2739,17 +2739,17 @@
         <v>2023</v>
       </c>
       <c r="D79" s="1" t="s">
-        <v>156</v>
+        <v>153</v>
       </c>
       <c r="E79" s="1" t="s">
-        <v>134</v>
+        <v>153</v>
       </c>
       <c r="F79" s="1"/>
       <c r="G79" s="1"/>
     </row>
     <row r="80" spans="1:7">
       <c r="A80" s="1" t="s">
-        <v>8</v>
+        <v>9</v>
       </c>
       <c r="B80" s="1" t="s">
         <v>81</v>
@@ -2758,10 +2758,10 @@
         <v>2023</v>
       </c>
       <c r="D80" s="1" t="s">
-        <v>154</v>
+        <v>156</v>
       </c>
       <c r="E80" s="1" t="s">
-        <v>154</v>
+        <v>134</v>
       </c>
       <c r="F80" s="1"/>
       <c r="G80" s="1"/>
@@ -2825,7 +2825,7 @@
     </row>
     <row r="84" spans="1:7">
       <c r="A84" s="1" t="s">
-        <v>8</v>
+        <v>14</v>
       </c>
       <c r="B84" s="1" t="s">
         <v>85</v>
@@ -2844,7 +2844,7 @@
     </row>
     <row r="85" spans="1:7">
       <c r="A85" s="1" t="s">
-        <v>14</v>
+        <v>8</v>
       </c>
       <c r="B85" s="1" t="s">
         <v>85</v>
@@ -2863,7 +2863,7 @@
     </row>
     <row r="86" spans="1:7">
       <c r="A86" s="1" t="s">
-        <v>12</v>
+        <v>9</v>
       </c>
       <c r="B86" s="1" t="s">
         <v>86</v>
@@ -2882,7 +2882,7 @@
     </row>
     <row r="87" spans="1:7">
       <c r="A87" s="1" t="s">
-        <v>9</v>
+        <v>7</v>
       </c>
       <c r="B87" s="1" t="s">
         <v>86</v>
@@ -2901,7 +2901,7 @@
     </row>
     <row r="88" spans="1:7">
       <c r="A88" s="1" t="s">
-        <v>7</v>
+        <v>12</v>
       </c>
       <c r="B88" s="1" t="s">
         <v>86</v>
@@ -2929,17 +2929,17 @@
         <v>2023</v>
       </c>
       <c r="D89" s="1" t="s">
-        <v>186</v>
+        <v>185</v>
       </c>
       <c r="E89" s="1" t="s">
-        <v>269</v>
+        <v>268</v>
       </c>
       <c r="F89" s="1"/>
       <c r="G89" s="1"/>
     </row>
     <row r="90" spans="1:7">
       <c r="A90" s="1" t="s">
-        <v>7</v>
+        <v>12</v>
       </c>
       <c r="B90" s="1" t="s">
         <v>87</v>
@@ -2951,14 +2951,14 @@
         <v>187</v>
       </c>
       <c r="E90" s="1" t="s">
-        <v>271</v>
+        <v>270</v>
       </c>
       <c r="F90" s="1"/>
       <c r="G90" s="1"/>
     </row>
     <row r="91" spans="1:7">
       <c r="A91" s="1" t="s">
-        <v>12</v>
+        <v>7</v>
       </c>
       <c r="B91" s="1" t="s">
         <v>87</v>
@@ -2967,10 +2967,10 @@
         <v>2023</v>
       </c>
       <c r="D91" s="1" t="s">
-        <v>185</v>
+        <v>186</v>
       </c>
       <c r="E91" s="1" t="s">
-        <v>268</v>
+        <v>271</v>
       </c>
       <c r="F91" s="1"/>
       <c r="G91" s="1"/>
@@ -3015,7 +3015,7 @@
     </row>
     <row r="94" spans="1:7">
       <c r="A94" s="1" t="s">
-        <v>7</v>
+        <v>8</v>
       </c>
       <c r="B94" s="1" t="s">
         <v>89</v>
@@ -3034,7 +3034,7 @@
     </row>
     <row r="95" spans="1:7">
       <c r="A95" s="1" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="B95" s="1" t="s">
         <v>89</v>
@@ -3053,7 +3053,7 @@
     </row>
     <row r="96" spans="1:7">
       <c r="A96" s="1" t="s">
-        <v>7</v>
+        <v>8</v>
       </c>
       <c r="B96" s="1" t="s">
         <v>90</v>
@@ -3072,7 +3072,7 @@
     </row>
     <row r="97" spans="1:7">
       <c r="A97" s="1" t="s">
-        <v>8</v>
+        <v>11</v>
       </c>
       <c r="B97" s="1" t="s">
         <v>90</v>
@@ -3091,7 +3091,7 @@
     </row>
     <row r="98" spans="1:7">
       <c r="A98" s="1" t="s">
-        <v>11</v>
+        <v>7</v>
       </c>
       <c r="B98" s="1" t="s">
         <v>90</v>
@@ -3129,7 +3129,7 @@
     </row>
     <row r="100" spans="1:7">
       <c r="A100" s="1" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="B100" s="1" t="s">
         <v>92</v>
@@ -3141,14 +3141,14 @@
         <v>196</v>
       </c>
       <c r="E100" s="1" t="s">
-        <v>196</v>
+        <v>272</v>
       </c>
       <c r="F100" s="1"/>
       <c r="G100" s="1"/>
     </row>
     <row r="101" spans="1:7">
       <c r="A101" s="1" t="s">
-        <v>7</v>
+        <v>8</v>
       </c>
       <c r="B101" s="1" t="s">
         <v>92</v>
@@ -3160,7 +3160,7 @@
         <v>197</v>
       </c>
       <c r="E101" s="1" t="s">
-        <v>272</v>
+        <v>197</v>
       </c>
       <c r="F101" s="1"/>
       <c r="G101" s="1"/>
@@ -3179,7 +3179,7 @@
         <v>198</v>
       </c>
       <c r="E102" s="1" t="s">
-        <v>225</v>
+        <v>224</v>
       </c>
       <c r="F102" s="1"/>
       <c r="G102" s="1"/>
@@ -3205,7 +3205,7 @@
     </row>
     <row r="104" spans="1:7">
       <c r="A104" s="1" t="s">
-        <v>7</v>
+        <v>9</v>
       </c>
       <c r="B104" s="1" t="s">
         <v>94</v>
@@ -3243,7 +3243,7 @@
     </row>
     <row r="106" spans="1:7">
       <c r="A106" s="1" t="s">
-        <v>9</v>
+        <v>7</v>
       </c>
       <c r="B106" s="1" t="s">
         <v>94</v>
@@ -3319,7 +3319,7 @@
     </row>
     <row r="110" spans="1:7">
       <c r="A110" s="1" t="s">
-        <v>7</v>
+        <v>8</v>
       </c>
       <c r="B110" s="1" t="s">
         <v>97</v>
@@ -3338,7 +3338,7 @@
     </row>
     <row r="111" spans="1:7">
       <c r="A111" s="1" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="B111" s="1" t="s">
         <v>97</v>
@@ -3376,7 +3376,7 @@
     </row>
     <row r="113" spans="1:7">
       <c r="A113" s="1" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="B113" s="1" t="s">
         <v>98</v>
@@ -3395,7 +3395,7 @@
     </row>
     <row r="114" spans="1:7">
       <c r="A114" s="1" t="s">
-        <v>7</v>
+        <v>10</v>
       </c>
       <c r="B114" s="1" t="s">
         <v>98</v>
@@ -3414,7 +3414,7 @@
     </row>
     <row r="115" spans="1:7">
       <c r="A115" s="1" t="s">
-        <v>10</v>
+        <v>12</v>
       </c>
       <c r="B115" s="1" t="s">
         <v>98</v>
@@ -3433,7 +3433,7 @@
     </row>
     <row r="116" spans="1:7">
       <c r="A116" s="1" t="s">
-        <v>12</v>
+        <v>9</v>
       </c>
       <c r="B116" s="1" t="s">
         <v>98</v>
@@ -3452,7 +3452,7 @@
     </row>
     <row r="117" spans="1:7">
       <c r="A117" s="1" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="B117" s="1" t="s">
         <v>98</v>
@@ -3471,7 +3471,7 @@
     </row>
     <row r="118" spans="1:7">
       <c r="A118" s="1" t="s">
-        <v>9</v>
+        <v>10</v>
       </c>
       <c r="B118" s="1" t="s">
         <v>99</v>
@@ -3483,14 +3483,14 @@
         <v>214</v>
       </c>
       <c r="E118" s="1" t="s">
-        <v>188</v>
+        <v>214</v>
       </c>
       <c r="F118" s="1"/>
       <c r="G118" s="1"/>
     </row>
     <row r="119" spans="1:7">
       <c r="A119" s="1" t="s">
-        <v>8</v>
+        <v>9</v>
       </c>
       <c r="B119" s="1" t="s">
         <v>99</v>
@@ -3502,14 +3502,14 @@
         <v>215</v>
       </c>
       <c r="E119" s="1" t="s">
-        <v>215</v>
+        <v>188</v>
       </c>
       <c r="F119" s="1"/>
       <c r="G119" s="1"/>
     </row>
     <row r="120" spans="1:7">
       <c r="A120" s="1" t="s">
-        <v>10</v>
+        <v>8</v>
       </c>
       <c r="B120" s="1" t="s">
         <v>99</v>
@@ -3528,7 +3528,7 @@
     </row>
     <row r="121" spans="1:7">
       <c r="A121" s="1" t="s">
-        <v>7</v>
+        <v>8</v>
       </c>
       <c r="B121" s="1" t="s">
         <v>100</v>
@@ -3537,17 +3537,17 @@
         <v>2023</v>
       </c>
       <c r="D121" s="1" t="s">
-        <v>217</v>
+        <v>216</v>
       </c>
       <c r="E121" s="1" t="s">
-        <v>277</v>
+        <v>216</v>
       </c>
       <c r="F121" s="1"/>
       <c r="G121" s="1"/>
     </row>
     <row r="122" spans="1:7">
       <c r="A122" s="1" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="B122" s="1" t="s">
         <v>100</v>
@@ -3556,17 +3556,17 @@
         <v>2023</v>
       </c>
       <c r="D122" s="1" t="s">
-        <v>215</v>
+        <v>217</v>
       </c>
       <c r="E122" s="1" t="s">
-        <v>215</v>
+        <v>277</v>
       </c>
       <c r="F122" s="1"/>
       <c r="G122" s="1"/>
     </row>
     <row r="123" spans="1:7">
       <c r="A123" s="1" t="s">
-        <v>12</v>
+        <v>10</v>
       </c>
       <c r="B123" s="1" t="s">
         <v>101</v>
@@ -3585,7 +3585,7 @@
     </row>
     <row r="124" spans="1:7">
       <c r="A124" s="1" t="s">
-        <v>10</v>
+        <v>12</v>
       </c>
       <c r="B124" s="1" t="s">
         <v>101</v>
@@ -3642,7 +3642,7 @@
     </row>
     <row r="127" spans="1:7">
       <c r="A127" s="1" t="s">
-        <v>7</v>
+        <v>8</v>
       </c>
       <c r="B127" s="1" t="s">
         <v>104</v>
@@ -3651,17 +3651,17 @@
         <v>2023</v>
       </c>
       <c r="D127" s="1" t="s">
-        <v>222</v>
+        <v>216</v>
       </c>
       <c r="E127" s="1" t="s">
-        <v>279</v>
+        <v>216</v>
       </c>
       <c r="F127" s="1"/>
       <c r="G127" s="1"/>
     </row>
     <row r="128" spans="1:7">
       <c r="A128" s="1" t="s">
-        <v>11</v>
+        <v>9</v>
       </c>
       <c r="B128" s="1" t="s">
         <v>104</v>
@@ -3670,17 +3670,17 @@
         <v>2023</v>
       </c>
       <c r="D128" s="1" t="s">
-        <v>223</v>
+        <v>188</v>
       </c>
       <c r="E128" s="1" t="s">
-        <v>280</v>
+        <v>188</v>
       </c>
       <c r="F128" s="1"/>
       <c r="G128" s="1"/>
     </row>
     <row r="129" spans="1:7">
       <c r="A129" s="1" t="s">
-        <v>9</v>
+        <v>7</v>
       </c>
       <c r="B129" s="1" t="s">
         <v>104</v>
@@ -3689,17 +3689,17 @@
         <v>2023</v>
       </c>
       <c r="D129" s="1" t="s">
-        <v>188</v>
+        <v>222</v>
       </c>
       <c r="E129" s="1" t="s">
-        <v>188</v>
+        <v>279</v>
       </c>
       <c r="F129" s="1"/>
       <c r="G129" s="1"/>
     </row>
     <row r="130" spans="1:7">
       <c r="A130" s="1" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
       <c r="B130" s="1" t="s">
         <v>104</v>
@@ -3708,17 +3708,17 @@
         <v>2023</v>
       </c>
       <c r="D130" s="1" t="s">
-        <v>224</v>
+        <v>223</v>
       </c>
       <c r="E130" s="1" t="s">
-        <v>224</v>
+        <v>280</v>
       </c>
       <c r="F130" s="1"/>
       <c r="G130" s="1"/>
     </row>
     <row r="131" spans="1:7">
       <c r="A131" s="1" t="s">
-        <v>8</v>
+        <v>10</v>
       </c>
       <c r="B131" s="1" t="s">
         <v>104</v>
@@ -3727,17 +3727,17 @@
         <v>2023</v>
       </c>
       <c r="D131" s="1" t="s">
-        <v>215</v>
+        <v>224</v>
       </c>
       <c r="E131" s="1" t="s">
-        <v>215</v>
+        <v>224</v>
       </c>
       <c r="F131" s="1"/>
       <c r="G131" s="1"/>
     </row>
     <row r="132" spans="1:7">
       <c r="A132" s="1" t="s">
-        <v>10</v>
+        <v>12</v>
       </c>
       <c r="B132" s="1" t="s">
         <v>104</v>
@@ -3756,7 +3756,7 @@
     </row>
     <row r="133" spans="1:7">
       <c r="A133" s="1" t="s">
-        <v>8</v>
+        <v>12</v>
       </c>
       <c r="B133" s="1" t="s">
         <v>105</v>
@@ -3775,7 +3775,7 @@
     </row>
     <row r="134" spans="1:7">
       <c r="A134" s="1" t="s">
-        <v>12</v>
+        <v>7</v>
       </c>
       <c r="B134" s="1" t="s">
         <v>105</v>
@@ -3787,14 +3787,14 @@
         <v>227</v>
       </c>
       <c r="E134" s="1" t="s">
-        <v>227</v>
+        <v>281</v>
       </c>
       <c r="F134" s="1"/>
       <c r="G134" s="1"/>
     </row>
     <row r="135" spans="1:7">
       <c r="A135" s="1" t="s">
-        <v>7</v>
+        <v>8</v>
       </c>
       <c r="B135" s="1" t="s">
         <v>105</v>
@@ -3806,7 +3806,7 @@
         <v>228</v>
       </c>
       <c r="E135" s="1" t="s">
-        <v>281</v>
+        <v>228</v>
       </c>
       <c r="F135" s="1"/>
       <c r="G135" s="1"/>
@@ -3889,7 +3889,7 @@
     </row>
     <row r="140" spans="1:7">
       <c r="A140" s="1" t="s">
-        <v>8</v>
+        <v>10</v>
       </c>
       <c r="B140" s="1" t="s">
         <v>110</v>
@@ -3898,17 +3898,17 @@
         <v>2023</v>
       </c>
       <c r="D140" s="1" t="s">
-        <v>215</v>
+        <v>224</v>
       </c>
       <c r="E140" s="1" t="s">
-        <v>215</v>
+        <v>224</v>
       </c>
       <c r="F140" s="1"/>
       <c r="G140" s="1"/>
     </row>
     <row r="141" spans="1:7">
       <c r="A141" s="1" t="s">
-        <v>10</v>
+        <v>8</v>
       </c>
       <c r="B141" s="1" t="s">
         <v>110</v>
@@ -3917,17 +3917,17 @@
         <v>2023</v>
       </c>
       <c r="D141" s="1" t="s">
-        <v>225</v>
+        <v>216</v>
       </c>
       <c r="E141" s="1" t="s">
-        <v>225</v>
+        <v>216</v>
       </c>
       <c r="F141" s="1"/>
       <c r="G141" s="1"/>
     </row>
     <row r="142" spans="1:7">
       <c r="A142" s="1" t="s">
-        <v>8</v>
+        <v>10</v>
       </c>
       <c r="B142" s="1" t="s">
         <v>111</v>
@@ -3936,17 +3936,17 @@
         <v>2023</v>
       </c>
       <c r="D142" s="1" t="s">
-        <v>196</v>
+        <v>218</v>
       </c>
       <c r="E142" s="1" t="s">
-        <v>196</v>
+        <v>218</v>
       </c>
       <c r="F142" s="1"/>
       <c r="G142" s="1"/>
     </row>
     <row r="143" spans="1:7">
       <c r="A143" s="1" t="s">
-        <v>10</v>
+        <v>8</v>
       </c>
       <c r="B143" s="1" t="s">
         <v>111</v>
@@ -3955,10 +3955,10 @@
         <v>2023</v>
       </c>
       <c r="D143" s="1" t="s">
-        <v>219</v>
+        <v>197</v>
       </c>
       <c r="E143" s="1" t="s">
-        <v>219</v>
+        <v>197</v>
       </c>
       <c r="F143" s="1"/>
       <c r="G143" s="1"/>
@@ -4050,10 +4050,10 @@
         <v>2023</v>
       </c>
       <c r="D148" s="1" t="s">
-        <v>215</v>
+        <v>216</v>
       </c>
       <c r="E148" s="1" t="s">
-        <v>215</v>
+        <v>216</v>
       </c>
       <c r="F148" s="1"/>
       <c r="G148" s="1"/>
@@ -4079,7 +4079,7 @@
     </row>
     <row r="150" spans="1:7">
       <c r="A150" s="1" t="s">
-        <v>8</v>
+        <v>9</v>
       </c>
       <c r="B150" s="1" t="s">
         <v>117</v>
@@ -4088,17 +4088,17 @@
         <v>2023</v>
       </c>
       <c r="D150" s="1" t="s">
-        <v>196</v>
+        <v>237</v>
       </c>
       <c r="E150" s="1" t="s">
-        <v>196</v>
+        <v>283</v>
       </c>
       <c r="F150" s="1"/>
       <c r="G150" s="1"/>
     </row>
     <row r="151" spans="1:7">
       <c r="A151" s="1" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="B151" s="1" t="s">
         <v>117</v>
@@ -4107,10 +4107,10 @@
         <v>2023</v>
       </c>
       <c r="D151" s="1" t="s">
-        <v>237</v>
+        <v>197</v>
       </c>
       <c r="E151" s="1" t="s">
-        <v>283</v>
+        <v>197</v>
       </c>
       <c r="F151" s="1"/>
       <c r="G151" s="1"/>
@@ -4250,7 +4250,7 @@
     </row>
     <row r="159" spans="1:7">
       <c r="A159" s="1" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="B159" s="1" t="s">
         <v>123</v>
@@ -4269,7 +4269,7 @@
     </row>
     <row r="160" spans="1:7">
       <c r="A160" s="1" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="B160" s="1" t="s">
         <v>123</v>
@@ -4288,7 +4288,7 @@
     </row>
     <row r="161" spans="1:7">
       <c r="A161" s="1" t="s">
-        <v>12</v>
+        <v>10</v>
       </c>
       <c r="B161" s="1" t="s">
         <v>123</v>
@@ -4326,7 +4326,7 @@
     </row>
     <row r="163" spans="1:7">
       <c r="A163" s="1" t="s">
-        <v>8</v>
+        <v>11</v>
       </c>
       <c r="B163" s="1" t="s">
         <v>123</v>
@@ -4345,7 +4345,7 @@
     </row>
     <row r="164" spans="1:7">
       <c r="A164" s="1" t="s">
-        <v>11</v>
+        <v>12</v>
       </c>
       <c r="B164" s="1" t="s">
         <v>123</v>

</xml_diff>

<commit_message>
Víc věcí v to-do a mírné zvýšení čitelnosti/škálovatelnosti
</commit_message>
<xml_diff>
--- a/results_xlsx/bez_garanta.xlsx
+++ b/results_xlsx/bez_garanta.xlsx
@@ -475,12 +475,12 @@
     <t>Úvod do molekulárních simulací</t>
   </si>
   <si>
+    <t>Bakalářská práce z chemie</t>
+  </si>
+  <si>
     <t>Bakalářská práce z fyziky</t>
   </si>
   <si>
-    <t>Bakalářská práce z chemie</t>
-  </si>
-  <si>
     <t>PVK - Elektronika II</t>
   </si>
   <si>
@@ -499,12 +499,12 @@
     <t>PVK - Automatizované měřící systémy</t>
   </si>
   <si>
+    <t>Diplomová práce z chemie</t>
+  </si>
+  <si>
     <t>Diplomová práce fyziky</t>
   </si>
   <si>
-    <t>Diplomová práce z chemie</t>
-  </si>
-  <si>
     <t>Obecná botanika</t>
   </si>
   <si>
@@ -571,36 +571,36 @@
     <t>Anglický jazyk pro doktorandy</t>
   </si>
   <si>
+    <t>SZZ - matematika s didaktikou</t>
+  </si>
+  <si>
     <t>SZZ - Geografie s didaktikou</t>
   </si>
   <si>
-    <t>SZZ - matematika s didaktikou</t>
-  </si>
-  <si>
     <t>SZZ - biologie s didaktikou</t>
   </si>
   <si>
     <t>Biologie</t>
   </si>
   <si>
+    <t>Aplikovaná fyzika</t>
+  </si>
+  <si>
     <t>Aplikovaná geografie - Cestovní ruch</t>
   </si>
   <si>
-    <t>Aplikovaná fyzika</t>
-  </si>
-  <si>
     <t>Softwarové systémy</t>
   </si>
   <si>
+    <t>Informační technologie</t>
+  </si>
+  <si>
+    <t>Nanotechnologie</t>
+  </si>
+  <si>
     <t>Aplikovaná geografie - Krajina a GIS</t>
   </si>
   <si>
-    <t>Nanotechnologie</t>
-  </si>
-  <si>
-    <t>Informační technologie</t>
-  </si>
-  <si>
     <t>Matematika s aplikacemi</t>
   </si>
   <si>
@@ -616,57 +616,57 @@
     <t>Statistika a zpracování dat</t>
   </si>
   <si>
+    <t>SZZ - Fyzika s didaktikou pro SŠ</t>
+  </si>
+  <si>
+    <t>Chemie a didaktika chemie pro SŠ</t>
+  </si>
+  <si>
+    <t>Geografie krajiny a GIS</t>
+  </si>
+  <si>
     <t>Biologie s didaktikou pro SŠ</t>
   </si>
   <si>
-    <t>Geografie krajiny a GIS</t>
-  </si>
-  <si>
-    <t>SZZ - Fyzika s didaktikou pro SŠ</t>
-  </si>
-  <si>
-    <t>Chemie a didaktika chemie pro SŠ</t>
-  </si>
-  <si>
     <t>Geografie venkova a sídel</t>
   </si>
   <si>
     <t>Regionální geografie a cestovní ruch</t>
   </si>
   <si>
+    <t>SZZ - numerická matematika</t>
+  </si>
+  <si>
+    <t>SZZ - Toxikologie a analýza škodlivin</t>
+  </si>
+  <si>
     <t>SZZ - Reg. geografie a reg. rozvoj Česka</t>
   </si>
   <si>
-    <t>SZZ - Toxikologie a analýza škodlivin</t>
-  </si>
-  <si>
-    <t>SZZ - numerická matematika</t>
+    <t>Matematika pro vzdělávání</t>
+  </si>
+  <si>
+    <t>Biologie pro vzdělávání</t>
+  </si>
+  <si>
+    <t>Chemie pro vzdělávání</t>
+  </si>
+  <si>
+    <t>Fyzika pro vzdělávání</t>
   </si>
   <si>
     <t>Geografie pro vzdělávání</t>
   </si>
   <si>
-    <t>Biologie pro vzdělávání</t>
-  </si>
-  <si>
-    <t>Fyzika pro vzdělávání</t>
-  </si>
-  <si>
-    <t>Chemie pro vzdělávání</t>
-  </si>
-  <si>
-    <t>Matematika pro vzdělávání</t>
+    <t>SZZ - Biologie</t>
+  </si>
+  <si>
+    <t>Fyzika</t>
   </si>
   <si>
     <t>Analytická chemie</t>
   </si>
   <si>
-    <t>SZZ - Biologie</t>
-  </si>
-  <si>
-    <t>Fyzika</t>
-  </si>
-  <si>
     <t>SZZ- Regionální geografie Evropy a světa</t>
   </si>
   <si>
@@ -682,27 +682,27 @@
     <t>SZZ - Fyzická geografie</t>
   </si>
   <si>
+    <t>Chemie</t>
+  </si>
+  <si>
+    <t>SZZ - Geografie</t>
+  </si>
+  <si>
     <t>Matematika</t>
   </si>
   <si>
     <t>SZZ - Informatika</t>
   </si>
   <si>
-    <t>SZZ - Geografie</t>
-  </si>
-  <si>
-    <t>Chemie</t>
+    <t>Matematická informatika</t>
+  </si>
+  <si>
+    <t>Elektronika a elektrotechnika</t>
   </si>
   <si>
     <t>SZZ - Obecná geografie</t>
   </si>
   <si>
-    <t>Matematická informatika</t>
-  </si>
-  <si>
-    <t>Elektronika a elektrotechnika</t>
-  </si>
-  <si>
     <t>SZZ - Sociální geografie</t>
   </si>
   <si>
@@ -739,36 +739,36 @@
     <t>Obecná fyzika a chemie</t>
   </si>
   <si>
+    <t>Nanotechnologie a nanomateriály</t>
+  </si>
+  <si>
     <t>Syntéza, technologie a analýza</t>
   </si>
   <si>
-    <t>Nanotechnologie a nanomateriály</t>
-  </si>
-  <si>
     <t>Aplikovaná informatika: povinný základ</t>
   </si>
   <si>
     <t>Sociální geografie a územní rozvoj</t>
   </si>
   <si>
+    <t>Učitelství fyziky pro střední školy</t>
+  </si>
+  <si>
+    <t>Učitelství geografie pro střední školy</t>
+  </si>
+  <si>
     <t>Učitelství chemie pro střední školy</t>
   </si>
   <si>
     <t>Učitelství biologie pro střední školy</t>
   </si>
   <si>
-    <t>Učitelství fyziky pro střední školy</t>
+    <t>Učitelství informatiky pro střední školy</t>
   </si>
   <si>
     <t>Učitelství matematiky pro střední školy</t>
   </si>
   <si>
-    <t>Učitelství geografie pro střední školy</t>
-  </si>
-  <si>
-    <t>Učitelství informatiky pro střední školy</t>
-  </si>
-  <si>
     <t>Teoretické základy datového inženýrství</t>
   </si>
   <si>
@@ -820,12 +820,12 @@
     <t>Chemické inženýrství</t>
   </si>
   <si>
+    <t>Matematika s didaktikou</t>
+  </si>
+  <si>
     <t>Geografie s didaktikou pro ZŠ</t>
   </si>
   <si>
-    <t>Matematika s didaktikou</t>
-  </si>
-  <si>
     <t>Biologie s didaktikou</t>
   </si>
   <si>
@@ -838,27 +838,27 @@
     <t>Fyzika s didaktikou pro SŠ</t>
   </si>
   <si>
+    <t>Numerická matematika</t>
+  </si>
+  <si>
+    <t>Toxikologie a analýza škodlivin</t>
+  </si>
+  <si>
     <t>Regionální geografie a regionální rozvoj Česka</t>
   </si>
   <si>
-    <t>Toxikologie a analýza škodlivin</t>
-  </si>
-  <si>
-    <t>Numerická matematika</t>
-  </si>
-  <si>
     <t>Regionální geografie Evropy a světa</t>
   </si>
   <si>
     <t>Fyzická geografie</t>
   </si>
   <si>
+    <t>Geografie</t>
+  </si>
+  <si>
     <t>Informatika</t>
   </si>
   <si>
-    <t>Geografie</t>
-  </si>
-  <si>
     <t>Obecná geografie</t>
   </si>
   <si>
@@ -871,10 +871,10 @@
     <t>Aplikovaná biologie, ekologie a ochrana biodiverzity</t>
   </si>
   <si>
+    <t>Nanotechnologie a nanomateriály, jejich příprava a charakterizace</t>
+  </si>
+  <si>
     <t>Syntéza, technologie a analýza chemických látek a materiálů</t>
-  </si>
-  <si>
-    <t>Nanotechnologie a nanomateriály, jejich příprava a charakterizace</t>
   </si>
 </sst>
 </file>
@@ -1514,7 +1514,7 @@
     </row>
     <row r="15" spans="1:7">
       <c r="A15" s="1" t="s">
-        <v>12</v>
+        <v>8</v>
       </c>
       <c r="B15" s="1" t="s">
         <v>27</v>
@@ -1533,7 +1533,7 @@
     </row>
     <row r="16" spans="1:7">
       <c r="A16" s="1" t="s">
-        <v>8</v>
+        <v>12</v>
       </c>
       <c r="B16" s="1" t="s">
         <v>27</v>
@@ -1552,7 +1552,7 @@
     </row>
     <row r="17" spans="1:7">
       <c r="A17" s="1" t="s">
-        <v>13</v>
+        <v>8</v>
       </c>
       <c r="B17" s="1" t="s">
         <v>28</v>
@@ -1571,7 +1571,7 @@
     </row>
     <row r="18" spans="1:7">
       <c r="A18" s="1" t="s">
-        <v>8</v>
+        <v>13</v>
       </c>
       <c r="B18" s="1" t="s">
         <v>28</v>
@@ -1590,7 +1590,7 @@
     </row>
     <row r="19" spans="1:7">
       <c r="A19" s="1" t="s">
-        <v>13</v>
+        <v>8</v>
       </c>
       <c r="B19" s="1" t="s">
         <v>29</v>
@@ -1609,7 +1609,7 @@
     </row>
     <row r="20" spans="1:7">
       <c r="A20" s="1" t="s">
-        <v>8</v>
+        <v>13</v>
       </c>
       <c r="B20" s="1" t="s">
         <v>29</v>
@@ -1628,7 +1628,7 @@
     </row>
     <row r="21" spans="1:7">
       <c r="A21" s="1" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
       <c r="B21" s="1" t="s">
         <v>30</v>
@@ -1647,7 +1647,7 @@
     </row>
     <row r="22" spans="1:7">
       <c r="A22" s="1" t="s">
-        <v>11</v>
+        <v>12</v>
       </c>
       <c r="B22" s="1" t="s">
         <v>30</v>
@@ -1666,7 +1666,7 @@
     </row>
     <row r="23" spans="1:7">
       <c r="A23" s="1" t="s">
-        <v>13</v>
+        <v>8</v>
       </c>
       <c r="B23" s="1" t="s">
         <v>31</v>
@@ -1685,7 +1685,7 @@
     </row>
     <row r="24" spans="1:7">
       <c r="A24" s="1" t="s">
-        <v>8</v>
+        <v>13</v>
       </c>
       <c r="B24" s="1" t="s">
         <v>31</v>
@@ -2008,7 +2008,7 @@
     </row>
     <row r="41" spans="1:7">
       <c r="A41" s="1" t="s">
-        <v>8</v>
+        <v>10</v>
       </c>
       <c r="B41" s="1" t="s">
         <v>47</v>
@@ -2027,7 +2027,7 @@
     </row>
     <row r="42" spans="1:7">
       <c r="A42" s="1" t="s">
-        <v>10</v>
+        <v>8</v>
       </c>
       <c r="B42" s="1" t="s">
         <v>47</v>
@@ -2179,7 +2179,7 @@
     </row>
     <row r="50" spans="1:7">
       <c r="A50" s="1" t="s">
-        <v>8</v>
+        <v>10</v>
       </c>
       <c r="B50" s="1" t="s">
         <v>54</v>
@@ -2191,14 +2191,14 @@
         <v>161</v>
       </c>
       <c r="E50" s="1" t="s">
-        <v>141</v>
+        <v>161</v>
       </c>
       <c r="F50" s="1"/>
       <c r="G50" s="1"/>
     </row>
     <row r="51" spans="1:7">
       <c r="A51" s="1" t="s">
-        <v>10</v>
+        <v>8</v>
       </c>
       <c r="B51" s="1" t="s">
         <v>54</v>
@@ -2210,7 +2210,7 @@
         <v>162</v>
       </c>
       <c r="E51" s="1" t="s">
-        <v>162</v>
+        <v>141</v>
       </c>
       <c r="F51" s="1"/>
       <c r="G51" s="1"/>
@@ -2578,7 +2578,7 @@
     </row>
     <row r="71" spans="1:7">
       <c r="A71" s="1" t="s">
-        <v>8</v>
+        <v>13</v>
       </c>
       <c r="B71" s="1" t="s">
         <v>74</v>
@@ -2597,7 +2597,7 @@
     </row>
     <row r="72" spans="1:7">
       <c r="A72" s="1" t="s">
-        <v>13</v>
+        <v>8</v>
       </c>
       <c r="B72" s="1" t="s">
         <v>74</v>
@@ -2739,10 +2739,10 @@
         <v>2023</v>
       </c>
       <c r="D79" s="1" t="s">
-        <v>153</v>
+        <v>154</v>
       </c>
       <c r="E79" s="1" t="s">
-        <v>153</v>
+        <v>154</v>
       </c>
       <c r="F79" s="1"/>
       <c r="G79" s="1"/>
@@ -2825,7 +2825,7 @@
     </row>
     <row r="84" spans="1:7">
       <c r="A84" s="1" t="s">
-        <v>8</v>
+        <v>14</v>
       </c>
       <c r="B84" s="1" t="s">
         <v>85</v>
@@ -2844,7 +2844,7 @@
     </row>
     <row r="85" spans="1:7">
       <c r="A85" s="1" t="s">
-        <v>14</v>
+        <v>8</v>
       </c>
       <c r="B85" s="1" t="s">
         <v>85</v>
@@ -2863,7 +2863,7 @@
     </row>
     <row r="86" spans="1:7">
       <c r="A86" s="1" t="s">
-        <v>7</v>
+        <v>12</v>
       </c>
       <c r="B86" s="1" t="s">
         <v>86</v>
@@ -2882,7 +2882,7 @@
     </row>
     <row r="87" spans="1:7">
       <c r="A87" s="1" t="s">
-        <v>12</v>
+        <v>7</v>
       </c>
       <c r="B87" s="1" t="s">
         <v>86</v>
@@ -2939,7 +2939,7 @@
     </row>
     <row r="90" spans="1:7">
       <c r="A90" s="1" t="s">
-        <v>7</v>
+        <v>12</v>
       </c>
       <c r="B90" s="1" t="s">
         <v>87</v>
@@ -2951,14 +2951,14 @@
         <v>185</v>
       </c>
       <c r="E90" s="1" t="s">
-        <v>271</v>
+        <v>268</v>
       </c>
       <c r="F90" s="1"/>
       <c r="G90" s="1"/>
     </row>
     <row r="91" spans="1:7">
       <c r="A91" s="1" t="s">
-        <v>12</v>
+        <v>7</v>
       </c>
       <c r="B91" s="1" t="s">
         <v>87</v>
@@ -2970,7 +2970,7 @@
         <v>186</v>
       </c>
       <c r="E91" s="1" t="s">
-        <v>269</v>
+        <v>271</v>
       </c>
       <c r="F91" s="1"/>
       <c r="G91" s="1"/>
@@ -2996,7 +2996,7 @@
     </row>
     <row r="93" spans="1:7">
       <c r="A93" s="1" t="s">
-        <v>7</v>
+        <v>8</v>
       </c>
       <c r="B93" s="1" t="s">
         <v>89</v>
@@ -3015,7 +3015,7 @@
     </row>
     <row r="94" spans="1:7">
       <c r="A94" s="1" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="B94" s="1" t="s">
         <v>89</v>
@@ -3053,7 +3053,7 @@
     </row>
     <row r="96" spans="1:7">
       <c r="A96" s="1" t="s">
-        <v>7</v>
+        <v>11</v>
       </c>
       <c r="B96" s="1" t="s">
         <v>90</v>
@@ -3091,7 +3091,7 @@
     </row>
     <row r="98" spans="1:7">
       <c r="A98" s="1" t="s">
-        <v>11</v>
+        <v>7</v>
       </c>
       <c r="B98" s="1" t="s">
         <v>90</v>
@@ -3141,7 +3141,7 @@
         <v>196</v>
       </c>
       <c r="E100" s="1" t="s">
-        <v>225</v>
+        <v>222</v>
       </c>
       <c r="F100" s="1"/>
       <c r="G100" s="1"/>
@@ -3205,7 +3205,7 @@
     </row>
     <row r="104" spans="1:7">
       <c r="A104" s="1" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="B104" s="1" t="s">
         <v>94</v>
@@ -3217,14 +3217,14 @@
         <v>200</v>
       </c>
       <c r="E104" s="1" t="s">
-        <v>200</v>
+        <v>273</v>
       </c>
       <c r="F104" s="1"/>
       <c r="G104" s="1"/>
     </row>
     <row r="105" spans="1:7">
       <c r="A105" s="1" t="s">
-        <v>7</v>
+        <v>10</v>
       </c>
       <c r="B105" s="1" t="s">
         <v>94</v>
@@ -3243,7 +3243,7 @@
     </row>
     <row r="106" spans="1:7">
       <c r="A106" s="1" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="B106" s="1" t="s">
         <v>94</v>
@@ -3255,14 +3255,14 @@
         <v>202</v>
       </c>
       <c r="E106" s="1" t="s">
-        <v>273</v>
+        <v>202</v>
       </c>
       <c r="F106" s="1"/>
       <c r="G106" s="1"/>
     </row>
     <row r="107" spans="1:7">
       <c r="A107" s="1" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="B107" s="1" t="s">
         <v>94</v>
@@ -3319,7 +3319,7 @@
     </row>
     <row r="110" spans="1:7">
       <c r="A110" s="1" t="s">
-        <v>7</v>
+        <v>8</v>
       </c>
       <c r="B110" s="1" t="s">
         <v>97</v>
@@ -3357,7 +3357,7 @@
     </row>
     <row r="112" spans="1:7">
       <c r="A112" s="1" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="B112" s="1" t="s">
         <v>97</v>
@@ -3376,7 +3376,7 @@
     </row>
     <row r="113" spans="1:7">
       <c r="A113" s="1" t="s">
-        <v>7</v>
+        <v>12</v>
       </c>
       <c r="B113" s="1" t="s">
         <v>98</v>
@@ -3414,7 +3414,7 @@
     </row>
     <row r="115" spans="1:7">
       <c r="A115" s="1" t="s">
-        <v>8</v>
+        <v>10</v>
       </c>
       <c r="B115" s="1" t="s">
         <v>98</v>
@@ -3433,7 +3433,7 @@
     </row>
     <row r="116" spans="1:7">
       <c r="A116" s="1" t="s">
-        <v>10</v>
+        <v>8</v>
       </c>
       <c r="B116" s="1" t="s">
         <v>98</v>
@@ -3452,7 +3452,7 @@
     </row>
     <row r="117" spans="1:7">
       <c r="A117" s="1" t="s">
-        <v>12</v>
+        <v>7</v>
       </c>
       <c r="B117" s="1" t="s">
         <v>98</v>
@@ -3471,7 +3471,7 @@
     </row>
     <row r="118" spans="1:7">
       <c r="A118" s="1" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="B118" s="1" t="s">
         <v>99</v>
@@ -3483,14 +3483,14 @@
         <v>214</v>
       </c>
       <c r="E118" s="1" t="s">
-        <v>214</v>
+        <v>188</v>
       </c>
       <c r="F118" s="1"/>
       <c r="G118" s="1"/>
     </row>
     <row r="119" spans="1:7">
       <c r="A119" s="1" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="B119" s="1" t="s">
         <v>99</v>
@@ -3502,14 +3502,14 @@
         <v>215</v>
       </c>
       <c r="E119" s="1" t="s">
-        <v>188</v>
+        <v>215</v>
       </c>
       <c r="F119" s="1"/>
       <c r="G119" s="1"/>
     </row>
     <row r="120" spans="1:7">
       <c r="A120" s="1" t="s">
-        <v>8</v>
+        <v>10</v>
       </c>
       <c r="B120" s="1" t="s">
         <v>99</v>
@@ -3528,7 +3528,7 @@
     </row>
     <row r="121" spans="1:7">
       <c r="A121" s="1" t="s">
-        <v>7</v>
+        <v>8</v>
       </c>
       <c r="B121" s="1" t="s">
         <v>100</v>
@@ -3537,17 +3537,17 @@
         <v>2023</v>
       </c>
       <c r="D121" s="1" t="s">
-        <v>217</v>
+        <v>215</v>
       </c>
       <c r="E121" s="1" t="s">
-        <v>277</v>
+        <v>215</v>
       </c>
       <c r="F121" s="1"/>
       <c r="G121" s="1"/>
     </row>
     <row r="122" spans="1:7">
       <c r="A122" s="1" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="B122" s="1" t="s">
         <v>100</v>
@@ -3556,10 +3556,10 @@
         <v>2023</v>
       </c>
       <c r="D122" s="1" t="s">
-        <v>216</v>
+        <v>217</v>
       </c>
       <c r="E122" s="1" t="s">
-        <v>216</v>
+        <v>277</v>
       </c>
       <c r="F122" s="1"/>
       <c r="G122" s="1"/>
@@ -3642,7 +3642,7 @@
     </row>
     <row r="127" spans="1:7">
       <c r="A127" s="1" t="s">
-        <v>12</v>
+        <v>10</v>
       </c>
       <c r="B127" s="1" t="s">
         <v>104</v>
@@ -3661,7 +3661,7 @@
     </row>
     <row r="128" spans="1:7">
       <c r="A128" s="1" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="B128" s="1" t="s">
         <v>104</v>
@@ -3670,17 +3670,17 @@
         <v>2023</v>
       </c>
       <c r="D128" s="1" t="s">
-        <v>188</v>
+        <v>215</v>
       </c>
       <c r="E128" s="1" t="s">
-        <v>188</v>
+        <v>215</v>
       </c>
       <c r="F128" s="1"/>
       <c r="G128" s="1"/>
     </row>
     <row r="129" spans="1:7">
       <c r="A129" s="1" t="s">
-        <v>11</v>
+        <v>7</v>
       </c>
       <c r="B129" s="1" t="s">
         <v>104</v>
@@ -3699,7 +3699,7 @@
     </row>
     <row r="130" spans="1:7">
       <c r="A130" s="1" t="s">
-        <v>8</v>
+        <v>12</v>
       </c>
       <c r="B130" s="1" t="s">
         <v>104</v>
@@ -3708,17 +3708,17 @@
         <v>2023</v>
       </c>
       <c r="D130" s="1" t="s">
-        <v>216</v>
+        <v>224</v>
       </c>
       <c r="E130" s="1" t="s">
-        <v>216</v>
+        <v>224</v>
       </c>
       <c r="F130" s="1"/>
       <c r="G130" s="1"/>
     </row>
     <row r="131" spans="1:7">
       <c r="A131" s="1" t="s">
-        <v>7</v>
+        <v>9</v>
       </c>
       <c r="B131" s="1" t="s">
         <v>104</v>
@@ -3727,17 +3727,17 @@
         <v>2023</v>
       </c>
       <c r="D131" s="1" t="s">
-        <v>224</v>
+        <v>188</v>
       </c>
       <c r="E131" s="1" t="s">
-        <v>280</v>
+        <v>188</v>
       </c>
       <c r="F131" s="1"/>
       <c r="G131" s="1"/>
     </row>
     <row r="132" spans="1:7">
       <c r="A132" s="1" t="s">
-        <v>10</v>
+        <v>11</v>
       </c>
       <c r="B132" s="1" t="s">
         <v>104</v>
@@ -3749,14 +3749,14 @@
         <v>225</v>
       </c>
       <c r="E132" s="1" t="s">
-        <v>225</v>
+        <v>280</v>
       </c>
       <c r="F132" s="1"/>
       <c r="G132" s="1"/>
     </row>
     <row r="133" spans="1:7">
       <c r="A133" s="1" t="s">
-        <v>7</v>
+        <v>12</v>
       </c>
       <c r="B133" s="1" t="s">
         <v>105</v>
@@ -3768,14 +3768,14 @@
         <v>226</v>
       </c>
       <c r="E133" s="1" t="s">
-        <v>281</v>
+        <v>226</v>
       </c>
       <c r="F133" s="1"/>
       <c r="G133" s="1"/>
     </row>
     <row r="134" spans="1:7">
       <c r="A134" s="1" t="s">
-        <v>12</v>
+        <v>8</v>
       </c>
       <c r="B134" s="1" t="s">
         <v>105</v>
@@ -3794,7 +3794,7 @@
     </row>
     <row r="135" spans="1:7">
       <c r="A135" s="1" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="B135" s="1" t="s">
         <v>105</v>
@@ -3806,7 +3806,7 @@
         <v>228</v>
       </c>
       <c r="E135" s="1" t="s">
-        <v>228</v>
+        <v>281</v>
       </c>
       <c r="F135" s="1"/>
       <c r="G135" s="1"/>
@@ -3898,10 +3898,10 @@
         <v>2023</v>
       </c>
       <c r="D140" s="1" t="s">
-        <v>216</v>
+        <v>215</v>
       </c>
       <c r="E140" s="1" t="s">
-        <v>216</v>
+        <v>215</v>
       </c>
       <c r="F140" s="1"/>
       <c r="G140" s="1"/>
@@ -3917,10 +3917,10 @@
         <v>2023</v>
       </c>
       <c r="D141" s="1" t="s">
-        <v>225</v>
+        <v>222</v>
       </c>
       <c r="E141" s="1" t="s">
-        <v>225</v>
+        <v>222</v>
       </c>
       <c r="F141" s="1"/>
       <c r="G141" s="1"/>
@@ -4050,10 +4050,10 @@
         <v>2023</v>
       </c>
       <c r="D148" s="1" t="s">
-        <v>216</v>
+        <v>215</v>
       </c>
       <c r="E148" s="1" t="s">
-        <v>216</v>
+        <v>215</v>
       </c>
       <c r="F148" s="1"/>
       <c r="G148" s="1"/>
@@ -4174,7 +4174,7 @@
     </row>
     <row r="155" spans="1:7">
       <c r="A155" s="1" t="s">
-        <v>10</v>
+        <v>8</v>
       </c>
       <c r="B155" s="1" t="s">
         <v>120</v>
@@ -4193,7 +4193,7 @@
     </row>
     <row r="156" spans="1:7">
       <c r="A156" s="1" t="s">
-        <v>8</v>
+        <v>10</v>
       </c>
       <c r="B156" s="1" t="s">
         <v>120</v>
@@ -4250,7 +4250,7 @@
     </row>
     <row r="159" spans="1:7">
       <c r="A159" s="1" t="s">
-        <v>10</v>
+        <v>8</v>
       </c>
       <c r="B159" s="1" t="s">
         <v>123</v>
@@ -4269,7 +4269,7 @@
     </row>
     <row r="160" spans="1:7">
       <c r="A160" s="1" t="s">
-        <v>9</v>
+        <v>7</v>
       </c>
       <c r="B160" s="1" t="s">
         <v>123</v>
@@ -4288,7 +4288,7 @@
     </row>
     <row r="161" spans="1:7">
       <c r="A161" s="1" t="s">
-        <v>8</v>
+        <v>10</v>
       </c>
       <c r="B161" s="1" t="s">
         <v>123</v>
@@ -4307,7 +4307,7 @@
     </row>
     <row r="162" spans="1:7">
       <c r="A162" s="1" t="s">
-        <v>12</v>
+        <v>9</v>
       </c>
       <c r="B162" s="1" t="s">
         <v>123</v>
@@ -4326,7 +4326,7 @@
     </row>
     <row r="163" spans="1:7">
       <c r="A163" s="1" t="s">
-        <v>7</v>
+        <v>11</v>
       </c>
       <c r="B163" s="1" t="s">
         <v>123</v>
@@ -4345,7 +4345,7 @@
     </row>
     <row r="164" spans="1:7">
       <c r="A164" s="1" t="s">
-        <v>11</v>
+        <v>12</v>
       </c>
       <c r="B164" s="1" t="s">
         <v>123</v>

</xml_diff>